<commit_message>
Finalizada serção "Decisão" sem revisão
</commit_message>
<xml_diff>
--- a/xls/Fases.xlsx
+++ b/xls/Fases.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fase_01" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -60,6 +61,45 @@
   </si>
   <si>
     <t>XBRL Consortium</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Total de Artigos</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Seleção nas Bases de Dados</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Remoção de Duplicatas e Livros</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Seleção por Titulo</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Seleção por Resumo (abstract)</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>Avaliação critérios de qualidade</t>
   </si>
 </sst>
 </file>
@@ -70,11 +110,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,6 +131,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,8 +209,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -160,19 +226,452 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="3200">
+                <a:latin typeface="Arial Black"/>
+              </a:rPr>
+              <a:t>Artigos Por Fase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$A$2:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1 Seleção nas Bases de Dados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total de Artigos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>407</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$A$3:$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F2 Remoção de Duplicatas e Livros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total de Artigos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$A$4:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F3 Seleção por Titulo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total de Artigos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$A$5:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F4 Seleção por Resumo (abstract)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total de Artigos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$A$6:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F5 Avaliação critérios de qualidade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total de Artigos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:axId val="15311557"/>
+        <c:axId val="65659233"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="15311557"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="65659233"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65659233"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="15311557"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>991440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>14760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>230760</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4433760" y="14760"/>
+        <a:ext cx="14866560" cy="7138080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13:D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -387,4 +886,102 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Inicio da apresentação final
</commit_message>
<xml_diff>
--- a/xls/Fases.xlsx
+++ b/xls/Fases.xlsx
@@ -133,11 +133,13 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="32"/>
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -289,7 +291,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -303,7 +305,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="3200">
+              <a:rPr b="1" sz="3200">
                 <a:latin typeface="Arial Black"/>
               </a:rPr>
               <a:t>Artigos Por Fase</a:t>
@@ -542,18 +544,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="15311557"/>
-        <c:axId val="65659233"/>
+        <c:axId val="56595617"/>
+        <c:axId val="28423132"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="15311557"/>
+        <c:axId val="56595617"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,14 +571,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65659233"/>
+        <c:crossAx val="28423132"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65659233"/>
+        <c:axId val="28423132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,8 +594,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15311557"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="56595617"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -631,16 +633,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>991440</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>230760</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -648,8 +650,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4433760" y="14760"/>
-        <a:ext cx="14866560" cy="7138080"/>
+        <a:off x="4460760" y="5760"/>
+        <a:ext cx="14866200" cy="7137720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -896,8 +898,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -971,7 +973,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>